<commit_message>
modified complete application fro immidart enterprise
</commit_message>
<xml_diff>
--- a/TestData/ImmidartTestData.xlsx
+++ b/TestData/ImmidartTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12345" windowHeight="6225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12030" windowHeight="6225"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>admin@immidart.com</t>
+    <t>password</t>
   </si>
   <si>
-    <t>password</t>
+    <t>admin@immidartqa.com</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +424,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to immidart lite from enterprise
</commit_message>
<xml_diff>
--- a/TestData/ImmidartTestData.xlsx
+++ b/TestData/ImmidartTestData.xlsx
@@ -23,10 +23,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>password</t>
+    <t>cm@ext462.com</t>
   </si>
   <si>
-    <t>admin@immidartqa.com</t>
+    <t>mtktB-P</t>
   </si>
 </sst>
 </file>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,16 +424,13 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>